<commit_message>
Fix Proportional and Integral Gain 800- modify the blue doc
</commit_message>
<xml_diff>
--- a/ER docs/ER-20018334_AK.xlsx
+++ b/ER docs/ER-20018334_AK.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Sensor Script\ER docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SensorScript\ER docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B9100857-B3FE-40A6-AE8A-654861FDC8D9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{15C9338F-6C52-4C40-8956-A414639DD65D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27525" windowHeight="11235" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,18 +27,18 @@
   </definedNames>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="tcunningham - Personal View" guid="{F6426E77-C675-444E-AC8D-180F66AA3059}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1351" windowHeight="765" activeSheetId="2"/>
+    <customWorkbookView name="MLupienski - Personal View" guid="{52161C46-7293-49CA-889B-1A1303EEF9B9}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1280" windowHeight="780" activeSheetId="1"/>
+    <customWorkbookView name="Tim Cunningham - Personal View" guid="{9D9E1FF7-61E9-4438-AEF2-B8A5765BA2AD}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1118" windowHeight="689" activeSheetId="1"/>
+    <customWorkbookView name="mcrisfield - Personal View" guid="{F566A51D-D37D-4C9A-A044-3E5B85972913}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1169" windowHeight="824" activeSheetId="5"/>
+    <customWorkbookView name="dgarnett - Personal View" guid="{7A3CD00D-9588-4788-B636-9D2E31C8323F}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1280" windowHeight="755" activeSheetId="1"/>
     <customWorkbookView name="gboney - Personal View" guid="{6531C455-43DF-4518-B2DB-CCE28F0AF57B}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1280" windowHeight="547" activeSheetId="5"/>
-    <customWorkbookView name="dgarnett - Personal View" guid="{7A3CD00D-9588-4788-B636-9D2E31C8323F}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1280" windowHeight="755" activeSheetId="1"/>
-    <customWorkbookView name="mcrisfield - Personal View" guid="{F566A51D-D37D-4C9A-A044-3E5B85972913}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1169" windowHeight="824" activeSheetId="5"/>
-    <customWorkbookView name="Tim Cunningham - Personal View" guid="{9D9E1FF7-61E9-4438-AEF2-B8A5765BA2AD}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1118" windowHeight="689" activeSheetId="1"/>
-    <customWorkbookView name="MLupienski - Personal View" guid="{52161C46-7293-49CA-889B-1A1303EEF9B9}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1280" windowHeight="780" activeSheetId="1"/>
-    <customWorkbookView name="tcunningham - Personal View" guid="{F6426E77-C675-444E-AC8D-180F66AA3059}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1351" windowHeight="765" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2780" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2780" uniqueCount="413">
   <si>
     <t>ID</t>
   </si>
@@ -1406,6 +1406,18 @@
   </si>
   <si>
     <t>TP</t>
+  </si>
+  <si>
+    <t>Proportional Gain 2200</t>
+  </si>
+  <si>
+    <t>Integral Gain 2200</t>
+  </si>
+  <si>
+    <t>Proportional Gain 800</t>
+  </si>
+  <si>
+    <t>Integral Gain 800</t>
   </si>
 </sst>
 </file>
@@ -2783,22 +2795,13 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2822,7 +2825,34 @@
     <xf numFmtId="1" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="30" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2842,24 +2872,6 @@
     </xf>
     <xf numFmtId="2" fontId="31" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="30" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="29">
@@ -3667,25 +3679,25 @@
   <sheetData>
     <row r="1" spans="1:47" ht="13.5" customHeight="1">
       <c r="A1" s="127"/>
-      <c r="B1" s="241" t="s">
+      <c r="B1" s="238" t="s">
         <v>264</v>
       </c>
-      <c r="C1" s="242"/>
-      <c r="D1" s="242"/>
-      <c r="E1" s="242"/>
-      <c r="F1" s="242"/>
-      <c r="G1" s="242"/>
-      <c r="H1" s="242"/>
-      <c r="I1" s="242"/>
-      <c r="J1" s="242"/>
-      <c r="K1" s="242"/>
-      <c r="L1" s="242"/>
-      <c r="M1" s="242"/>
-      <c r="N1" s="242"/>
-      <c r="O1" s="242"/>
-      <c r="P1" s="242"/>
-      <c r="Q1" s="242"/>
-      <c r="R1" s="243"/>
+      <c r="C1" s="239"/>
+      <c r="D1" s="239"/>
+      <c r="E1" s="239"/>
+      <c r="F1" s="239"/>
+      <c r="G1" s="239"/>
+      <c r="H1" s="239"/>
+      <c r="I1" s="239"/>
+      <c r="J1" s="239"/>
+      <c r="K1" s="239"/>
+      <c r="L1" s="239"/>
+      <c r="M1" s="239"/>
+      <c r="N1" s="239"/>
+      <c r="O1" s="239"/>
+      <c r="P1" s="239"/>
+      <c r="Q1" s="239"/>
+      <c r="R1" s="240"/>
       <c r="S1" s="128"/>
       <c r="T1" s="129"/>
       <c r="U1" s="129"/>
@@ -3718,23 +3730,23 @@
     </row>
     <row r="2" spans="1:47" ht="13.5" customHeight="1" thickBot="1">
       <c r="A2" s="135"/>
-      <c r="B2" s="244"/>
-      <c r="C2" s="245"/>
-      <c r="D2" s="245"/>
-      <c r="E2" s="245"/>
-      <c r="F2" s="245"/>
-      <c r="G2" s="245"/>
-      <c r="H2" s="245"/>
-      <c r="I2" s="245"/>
-      <c r="J2" s="245"/>
-      <c r="K2" s="245"/>
-      <c r="L2" s="245"/>
-      <c r="M2" s="245"/>
-      <c r="N2" s="245"/>
-      <c r="O2" s="245"/>
-      <c r="P2" s="245"/>
-      <c r="Q2" s="245"/>
-      <c r="R2" s="246"/>
+      <c r="B2" s="241"/>
+      <c r="C2" s="242"/>
+      <c r="D2" s="242"/>
+      <c r="E2" s="242"/>
+      <c r="F2" s="242"/>
+      <c r="G2" s="242"/>
+      <c r="H2" s="242"/>
+      <c r="I2" s="242"/>
+      <c r="J2" s="242"/>
+      <c r="K2" s="242"/>
+      <c r="L2" s="242"/>
+      <c r="M2" s="242"/>
+      <c r="N2" s="242"/>
+      <c r="O2" s="242"/>
+      <c r="P2" s="242"/>
+      <c r="Q2" s="242"/>
+      <c r="R2" s="243"/>
       <c r="S2" s="31"/>
       <c r="AA2" s="33"/>
       <c r="AB2" s="33"/>
@@ -3969,13 +3981,13 @@
       <c r="O9" s="33" t="s">
         <v>265</v>
       </c>
-      <c r="Z9" s="238" t="s">
+      <c r="Z9" s="247" t="s">
         <v>158</v>
       </c>
-      <c r="AA9" s="238"/>
-      <c r="AB9" s="238"/>
-      <c r="AC9" s="238"/>
-      <c r="AD9" s="238"/>
+      <c r="AA9" s="247"/>
+      <c r="AB9" s="247"/>
+      <c r="AC9" s="247"/>
+      <c r="AD9" s="247"/>
       <c r="AK9" s="30"/>
       <c r="AL9" s="32"/>
       <c r="AM9" s="30"/>
@@ -4005,11 +4017,11 @@
       <c r="O10" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="Z10" s="238"/>
-      <c r="AA10" s="238"/>
-      <c r="AB10" s="238"/>
-      <c r="AC10" s="238"/>
-      <c r="AD10" s="238"/>
+      <c r="Z10" s="247"/>
+      <c r="AA10" s="247"/>
+      <c r="AB10" s="247"/>
+      <c r="AC10" s="247"/>
+      <c r="AD10" s="247"/>
       <c r="AK10" s="30"/>
       <c r="AL10" s="32"/>
       <c r="AM10" s="30"/>
@@ -4158,128 +4170,128 @@
       <c r="AU15" s="121"/>
     </row>
     <row r="16" spans="1:47" ht="13.5" customHeight="1">
-      <c r="A16" s="248" t="s">
+      <c r="A16" s="235" t="s">
         <v>263</v>
       </c>
-      <c r="B16" s="235" t="s">
+      <c r="B16" s="236" t="s">
         <v>253</v>
       </c>
-      <c r="C16" s="235" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="235" t="s">
+      <c r="C16" s="236" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="236" t="s">
         <v>99</v>
       </c>
-      <c r="E16" s="235" t="s">
+      <c r="E16" s="236" t="s">
         <v>283</v>
       </c>
-      <c r="F16" s="235" t="s">
+      <c r="F16" s="236" t="s">
         <v>284</v>
       </c>
-      <c r="G16" s="235" t="s">
+      <c r="G16" s="236" t="s">
         <v>285</v>
       </c>
-      <c r="H16" s="235" t="s">
+      <c r="H16" s="236" t="s">
         <v>145</v>
       </c>
-      <c r="I16" s="235" t="s">
+      <c r="I16" s="236" t="s">
         <v>144</v>
       </c>
-      <c r="J16" s="235" t="s">
+      <c r="J16" s="236" t="s">
         <v>269</v>
       </c>
-      <c r="K16" s="235" t="s">
+      <c r="K16" s="236" t="s">
         <v>270</v>
       </c>
-      <c r="L16" s="247" t="s">
+      <c r="L16" s="244" t="s">
         <v>271</v>
       </c>
-      <c r="M16" s="235" t="s">
+      <c r="M16" s="236" t="s">
         <v>272</v>
       </c>
-      <c r="N16" s="235" t="s">
+      <c r="N16" s="236" t="s">
         <v>267</v>
       </c>
-      <c r="O16" s="235" t="s">
+      <c r="O16" s="236" t="s">
         <v>268</v>
       </c>
-      <c r="P16" s="235" t="s">
+      <c r="P16" s="236" t="s">
         <v>146</v>
       </c>
-      <c r="Q16" s="235" t="s">
+      <c r="Q16" s="236" t="s">
         <v>146</v>
       </c>
-      <c r="R16" s="235" t="s">
+      <c r="R16" s="236" t="s">
         <v>274</v>
       </c>
-      <c r="S16" s="239" t="s">
+      <c r="S16" s="237" t="s">
         <v>147</v>
       </c>
-      <c r="T16" s="239" t="s">
+      <c r="T16" s="237" t="s">
         <v>303</v>
       </c>
-      <c r="U16" s="239" t="s">
+      <c r="U16" s="237" t="s">
         <v>304</v>
       </c>
-      <c r="V16" s="239" t="s">
+      <c r="V16" s="237" t="s">
         <v>306</v>
       </c>
-      <c r="W16" s="239" t="s">
+      <c r="W16" s="237" t="s">
         <v>307</v>
       </c>
-      <c r="X16" s="239" t="s">
+      <c r="X16" s="237" t="s">
         <v>309</v>
       </c>
-      <c r="Y16" s="239" t="s">
+      <c r="Y16" s="237" t="s">
         <v>334</v>
       </c>
-      <c r="Z16" s="240" t="s">
+      <c r="Z16" s="248" t="s">
         <v>135</v>
       </c>
-      <c r="AA16" s="235" t="s">
+      <c r="AA16" s="236" t="s">
         <v>136</v>
       </c>
-      <c r="AB16" s="235" t="s">
+      <c r="AB16" s="236" t="s">
         <v>137</v>
       </c>
-      <c r="AC16" s="235" t="s">
+      <c r="AC16" s="236" t="s">
         <v>138</v>
       </c>
-      <c r="AD16" s="235" t="s">
+      <c r="AD16" s="236" t="s">
         <v>139</v>
       </c>
-      <c r="AE16" s="235" t="s">
+      <c r="AE16" s="236" t="s">
         <v>140</v>
       </c>
-      <c r="AF16" s="235" t="s">
+      <c r="AF16" s="236" t="s">
         <v>141</v>
       </c>
-      <c r="AG16" s="235" t="s">
+      <c r="AG16" s="236" t="s">
         <v>142</v>
       </c>
-      <c r="AH16" s="235" t="s">
+      <c r="AH16" s="236" t="s">
         <v>143</v>
       </c>
-      <c r="AI16" s="235" t="s">
+      <c r="AI16" s="236" t="s">
         <v>330</v>
       </c>
-      <c r="AJ16" s="235"/>
-      <c r="AK16" s="235" t="s">
+      <c r="AJ16" s="236"/>
+      <c r="AK16" s="236" t="s">
         <v>282</v>
       </c>
-      <c r="AL16" s="236" t="s">
+      <c r="AL16" s="246" t="s">
         <v>68</v>
       </c>
-      <c r="AM16" s="236" t="s">
+      <c r="AM16" s="246" t="s">
         <v>69</v>
       </c>
-      <c r="AN16" s="236" t="s">
+      <c r="AN16" s="246" t="s">
         <v>159</v>
       </c>
-      <c r="AO16" s="236" t="s">
+      <c r="AO16" s="246" t="s">
         <v>160</v>
       </c>
-      <c r="AP16" s="237" t="s">
+      <c r="AP16" s="245" t="s">
         <v>108</v>
       </c>
       <c r="AQ16" s="42"/>
@@ -4287,155 +4299,155 @@
       <c r="AU16" s="121"/>
     </row>
     <row r="17" spans="1:47" ht="13.5" customHeight="1">
-      <c r="A17" s="248"/>
-      <c r="B17" s="235"/>
-      <c r="C17" s="235"/>
-      <c r="D17" s="235"/>
-      <c r="E17" s="235"/>
-      <c r="F17" s="235"/>
-      <c r="G17" s="235"/>
-      <c r="H17" s="235"/>
-      <c r="I17" s="235"/>
-      <c r="J17" s="235"/>
-      <c r="K17" s="235"/>
-      <c r="L17" s="247"/>
-      <c r="M17" s="235"/>
-      <c r="N17" s="235"/>
-      <c r="O17" s="235"/>
-      <c r="P17" s="235"/>
-      <c r="Q17" s="235"/>
-      <c r="R17" s="235"/>
-      <c r="S17" s="239"/>
-      <c r="T17" s="239"/>
-      <c r="U17" s="239"/>
-      <c r="V17" s="239"/>
-      <c r="W17" s="239"/>
-      <c r="X17" s="239"/>
-      <c r="Y17" s="239"/>
-      <c r="Z17" s="240"/>
-      <c r="AA17" s="235"/>
-      <c r="AB17" s="235"/>
-      <c r="AC17" s="235"/>
-      <c r="AD17" s="235"/>
-      <c r="AE17" s="235"/>
-      <c r="AF17" s="235"/>
-      <c r="AG17" s="235"/>
-      <c r="AH17" s="235"/>
-      <c r="AI17" s="235"/>
-      <c r="AJ17" s="235"/>
-      <c r="AK17" s="235"/>
-      <c r="AL17" s="236"/>
-      <c r="AM17" s="236"/>
-      <c r="AN17" s="236"/>
-      <c r="AO17" s="236"/>
-      <c r="AP17" s="237"/>
+      <c r="A17" s="235"/>
+      <c r="B17" s="236"/>
+      <c r="C17" s="236"/>
+      <c r="D17" s="236"/>
+      <c r="E17" s="236"/>
+      <c r="F17" s="236"/>
+      <c r="G17" s="236"/>
+      <c r="H17" s="236"/>
+      <c r="I17" s="236"/>
+      <c r="J17" s="236"/>
+      <c r="K17" s="236"/>
+      <c r="L17" s="244"/>
+      <c r="M17" s="236"/>
+      <c r="N17" s="236"/>
+      <c r="O17" s="236"/>
+      <c r="P17" s="236"/>
+      <c r="Q17" s="236"/>
+      <c r="R17" s="236"/>
+      <c r="S17" s="237"/>
+      <c r="T17" s="237"/>
+      <c r="U17" s="237"/>
+      <c r="V17" s="237"/>
+      <c r="W17" s="237"/>
+      <c r="X17" s="237"/>
+      <c r="Y17" s="237"/>
+      <c r="Z17" s="248"/>
+      <c r="AA17" s="236"/>
+      <c r="AB17" s="236"/>
+      <c r="AC17" s="236"/>
+      <c r="AD17" s="236"/>
+      <c r="AE17" s="236"/>
+      <c r="AF17" s="236"/>
+      <c r="AG17" s="236"/>
+      <c r="AH17" s="236"/>
+      <c r="AI17" s="236"/>
+      <c r="AJ17" s="236"/>
+      <c r="AK17" s="236"/>
+      <c r="AL17" s="246"/>
+      <c r="AM17" s="246"/>
+      <c r="AN17" s="246"/>
+      <c r="AO17" s="246"/>
+      <c r="AP17" s="245"/>
       <c r="AQ17" s="42"/>
       <c r="AT17" s="136"/>
       <c r="AU17" s="121"/>
     </row>
     <row r="18" spans="1:47" ht="13.5" customHeight="1">
-      <c r="A18" s="248"/>
-      <c r="B18" s="235"/>
-      <c r="C18" s="235"/>
-      <c r="D18" s="235"/>
-      <c r="E18" s="235"/>
-      <c r="F18" s="235"/>
-      <c r="G18" s="235"/>
-      <c r="H18" s="235"/>
-      <c r="I18" s="235"/>
-      <c r="J18" s="235"/>
-      <c r="K18" s="235"/>
-      <c r="L18" s="247"/>
-      <c r="M18" s="235"/>
-      <c r="N18" s="235"/>
-      <c r="O18" s="235"/>
-      <c r="P18" s="235"/>
-      <c r="Q18" s="235"/>
-      <c r="R18" s="235"/>
-      <c r="S18" s="239"/>
-      <c r="T18" s="239"/>
-      <c r="U18" s="239"/>
-      <c r="V18" s="239"/>
-      <c r="W18" s="239"/>
-      <c r="X18" s="239"/>
-      <c r="Y18" s="239"/>
-      <c r="Z18" s="240"/>
-      <c r="AA18" s="235"/>
-      <c r="AB18" s="235"/>
-      <c r="AC18" s="235"/>
-      <c r="AD18" s="235"/>
-      <c r="AE18" s="235"/>
-      <c r="AF18" s="235"/>
-      <c r="AG18" s="235"/>
-      <c r="AH18" s="235"/>
-      <c r="AI18" s="235" t="s">
+      <c r="A18" s="235"/>
+      <c r="B18" s="236"/>
+      <c r="C18" s="236"/>
+      <c r="D18" s="236"/>
+      <c r="E18" s="236"/>
+      <c r="F18" s="236"/>
+      <c r="G18" s="236"/>
+      <c r="H18" s="236"/>
+      <c r="I18" s="236"/>
+      <c r="J18" s="236"/>
+      <c r="K18" s="236"/>
+      <c r="L18" s="244"/>
+      <c r="M18" s="236"/>
+      <c r="N18" s="236"/>
+      <c r="O18" s="236"/>
+      <c r="P18" s="236"/>
+      <c r="Q18" s="236"/>
+      <c r="R18" s="236"/>
+      <c r="S18" s="237"/>
+      <c r="T18" s="237"/>
+      <c r="U18" s="237"/>
+      <c r="V18" s="237"/>
+      <c r="W18" s="237"/>
+      <c r="X18" s="237"/>
+      <c r="Y18" s="237"/>
+      <c r="Z18" s="248"/>
+      <c r="AA18" s="236"/>
+      <c r="AB18" s="236"/>
+      <c r="AC18" s="236"/>
+      <c r="AD18" s="236"/>
+      <c r="AE18" s="236"/>
+      <c r="AF18" s="236"/>
+      <c r="AG18" s="236"/>
+      <c r="AH18" s="236"/>
+      <c r="AI18" s="236" t="s">
         <v>322</v>
       </c>
-      <c r="AJ18" s="235" t="s">
+      <c r="AJ18" s="236" t="s">
         <v>323</v>
       </c>
-      <c r="AK18" s="235"/>
-      <c r="AL18" s="236"/>
-      <c r="AM18" s="236"/>
-      <c r="AN18" s="236"/>
-      <c r="AO18" s="236"/>
-      <c r="AP18" s="237"/>
+      <c r="AK18" s="236"/>
+      <c r="AL18" s="246"/>
+      <c r="AM18" s="246"/>
+      <c r="AN18" s="246"/>
+      <c r="AO18" s="246"/>
+      <c r="AP18" s="245"/>
       <c r="AQ18" s="42"/>
       <c r="AT18" s="136"/>
       <c r="AU18" s="121"/>
     </row>
     <row r="19" spans="1:47" ht="13.5" customHeight="1">
-      <c r="A19" s="248"/>
-      <c r="B19" s="235"/>
-      <c r="C19" s="235"/>
-      <c r="D19" s="235"/>
-      <c r="E19" s="235"/>
-      <c r="F19" s="235"/>
-      <c r="G19" s="235"/>
-      <c r="H19" s="235"/>
-      <c r="I19" s="235"/>
-      <c r="J19" s="235"/>
-      <c r="K19" s="235"/>
-      <c r="L19" s="247"/>
-      <c r="M19" s="235"/>
-      <c r="N19" s="235"/>
-      <c r="O19" s="235"/>
-      <c r="P19" s="235"/>
-      <c r="Q19" s="235"/>
-      <c r="R19" s="235"/>
-      <c r="S19" s="239"/>
-      <c r="T19" s="239"/>
-      <c r="U19" s="239"/>
-      <c r="V19" s="239"/>
-      <c r="W19" s="239"/>
-      <c r="X19" s="239"/>
-      <c r="Y19" s="239"/>
-      <c r="Z19" s="240"/>
-      <c r="AA19" s="235"/>
-      <c r="AB19" s="235"/>
-      <c r="AC19" s="235"/>
-      <c r="AD19" s="235"/>
-      <c r="AE19" s="235"/>
-      <c r="AF19" s="235"/>
-      <c r="AG19" s="235"/>
-      <c r="AH19" s="235"/>
-      <c r="AI19" s="235"/>
-      <c r="AJ19" s="235"/>
-      <c r="AK19" s="235"/>
-      <c r="AL19" s="236"/>
-      <c r="AM19" s="236"/>
-      <c r="AN19" s="236"/>
-      <c r="AO19" s="236"/>
-      <c r="AP19" s="237"/>
+      <c r="A19" s="235"/>
+      <c r="B19" s="236"/>
+      <c r="C19" s="236"/>
+      <c r="D19" s="236"/>
+      <c r="E19" s="236"/>
+      <c r="F19" s="236"/>
+      <c r="G19" s="236"/>
+      <c r="H19" s="236"/>
+      <c r="I19" s="236"/>
+      <c r="J19" s="236"/>
+      <c r="K19" s="236"/>
+      <c r="L19" s="244"/>
+      <c r="M19" s="236"/>
+      <c r="N19" s="236"/>
+      <c r="O19" s="236"/>
+      <c r="P19" s="236"/>
+      <c r="Q19" s="236"/>
+      <c r="R19" s="236"/>
+      <c r="S19" s="237"/>
+      <c r="T19" s="237"/>
+      <c r="U19" s="237"/>
+      <c r="V19" s="237"/>
+      <c r="W19" s="237"/>
+      <c r="X19" s="237"/>
+      <c r="Y19" s="237"/>
+      <c r="Z19" s="248"/>
+      <c r="AA19" s="236"/>
+      <c r="AB19" s="236"/>
+      <c r="AC19" s="236"/>
+      <c r="AD19" s="236"/>
+      <c r="AE19" s="236"/>
+      <c r="AF19" s="236"/>
+      <c r="AG19" s="236"/>
+      <c r="AH19" s="236"/>
+      <c r="AI19" s="236"/>
+      <c r="AJ19" s="236"/>
+      <c r="AK19" s="236"/>
+      <c r="AL19" s="246"/>
+      <c r="AM19" s="246"/>
+      <c r="AN19" s="246"/>
+      <c r="AO19" s="246"/>
+      <c r="AP19" s="245"/>
       <c r="AQ19" s="42"/>
       <c r="AT19" s="136"/>
       <c r="AU19" s="121"/>
     </row>
     <row r="20" spans="1:47" ht="13.5" customHeight="1">
-      <c r="A20" s="248"/>
-      <c r="B20" s="235"/>
-      <c r="C20" s="235"/>
-      <c r="D20" s="235"/>
+      <c r="A20" s="235"/>
+      <c r="B20" s="236"/>
+      <c r="C20" s="236"/>
+      <c r="D20" s="236"/>
       <c r="E20" s="43" t="s">
         <v>287</v>
       </c>
@@ -4478,7 +4490,7 @@
       <c r="R20" s="43" t="s">
         <v>276</v>
       </c>
-      <c r="S20" s="239"/>
+      <c r="S20" s="237"/>
       <c r="T20" s="8" t="s">
         <v>151</v>
       </c>
@@ -4491,36 +4503,36 @@
       <c r="W20" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="X20" s="239"/>
-      <c r="Y20" s="239"/>
-      <c r="Z20" s="240"/>
-      <c r="AA20" s="235"/>
-      <c r="AB20" s="235"/>
-      <c r="AC20" s="235"/>
-      <c r="AD20" s="235"/>
-      <c r="AE20" s="235"/>
-      <c r="AF20" s="235"/>
-      <c r="AG20" s="235"/>
-      <c r="AH20" s="235"/>
-      <c r="AI20" s="235"/>
-      <c r="AJ20" s="235"/>
-      <c r="AK20" s="235"/>
-      <c r="AL20" s="236"/>
-      <c r="AM20" s="236"/>
-      <c r="AN20" s="236"/>
-      <c r="AO20" s="236"/>
-      <c r="AP20" s="237"/>
+      <c r="X20" s="237"/>
+      <c r="Y20" s="237"/>
+      <c r="Z20" s="248"/>
+      <c r="AA20" s="236"/>
+      <c r="AB20" s="236"/>
+      <c r="AC20" s="236"/>
+      <c r="AD20" s="236"/>
+      <c r="AE20" s="236"/>
+      <c r="AF20" s="236"/>
+      <c r="AG20" s="236"/>
+      <c r="AH20" s="236"/>
+      <c r="AI20" s="236"/>
+      <c r="AJ20" s="236"/>
+      <c r="AK20" s="236"/>
+      <c r="AL20" s="246"/>
+      <c r="AM20" s="246"/>
+      <c r="AN20" s="246"/>
+      <c r="AO20" s="246"/>
+      <c r="AP20" s="245"/>
       <c r="AQ20" s="42"/>
       <c r="AT20" s="136"/>
       <c r="AU20" s="121"/>
     </row>
     <row r="21" spans="1:47" s="32" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A21" s="248"/>
-      <c r="B21" s="235"/>
+      <c r="A21" s="235"/>
+      <c r="B21" s="236"/>
       <c r="C21" s="43">
         <v>3019</v>
       </c>
-      <c r="D21" s="235"/>
+      <c r="D21" s="236"/>
       <c r="E21" s="43">
         <v>407</v>
       </c>
@@ -4596,11 +4608,11 @@
       <c r="AK21" s="43">
         <v>1069</v>
       </c>
-      <c r="AL21" s="236"/>
-      <c r="AM21" s="236"/>
-      <c r="AN21" s="236"/>
-      <c r="AO21" s="236"/>
-      <c r="AP21" s="237"/>
+      <c r="AL21" s="246"/>
+      <c r="AM21" s="246"/>
+      <c r="AN21" s="246"/>
+      <c r="AO21" s="246"/>
+      <c r="AP21" s="245"/>
       <c r="AQ21" s="42"/>
       <c r="AT21" s="137"/>
       <c r="AU21" s="122"/>
@@ -24329,8 +24341,18 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6531C455-43DF-4518-B2DB-CCE28F0AF57B}" showRuler="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <customSheetView guid="{F6426E77-C675-444E-AC8D-180F66AA3059}" showRuler="0">
+      <selection activeCell="G5" sqref="G5"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{52161C46-7293-49CA-889B-1A1303EEF9B9}" showRuler="0" topLeftCell="A23">
+      <selection activeCell="A31" sqref="A31"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{F566A51D-D37D-4C9A-A044-3E5B85972913}" showRuler="0">
+      <selection activeCell="B16" sqref="B16"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
@@ -24339,48 +24361,18 @@
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{F566A51D-D37D-4C9A-A044-3E5B85972913}" showRuler="0">
-      <selection activeCell="B16" sqref="B16"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{52161C46-7293-49CA-889B-1A1303EEF9B9}" showRuler="0" topLeftCell="A23">
-      <selection activeCell="A31" sqref="A31"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{F6426E77-C675-444E-AC8D-180F66AA3059}" showRuler="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <customSheetView guid="{6531C455-43DF-4518-B2DB-CCE28F0AF57B}" showRuler="0">
+      <selection activeCell="L24" sqref="L24"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="46">
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="P16:P19"/>
-    <mergeCell ref="O16:O19"/>
-    <mergeCell ref="N16:N19"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="G16:G19"/>
-    <mergeCell ref="D16:D21"/>
-    <mergeCell ref="K16:K19"/>
-    <mergeCell ref="J16:J19"/>
-    <mergeCell ref="I16:I19"/>
-    <mergeCell ref="C16:C20"/>
-    <mergeCell ref="Q16:Q19"/>
-    <mergeCell ref="X16:X20"/>
-    <mergeCell ref="B1:R2"/>
-    <mergeCell ref="U16:U19"/>
-    <mergeCell ref="R16:R19"/>
-    <mergeCell ref="B16:B21"/>
-    <mergeCell ref="M16:M19"/>
-    <mergeCell ref="L16:L19"/>
-    <mergeCell ref="F16:F19"/>
-    <mergeCell ref="E16:E19"/>
-    <mergeCell ref="T16:T19"/>
-    <mergeCell ref="S16:S20"/>
-    <mergeCell ref="V16:V19"/>
-    <mergeCell ref="W16:W19"/>
+    <mergeCell ref="AJ18:AJ19"/>
+    <mergeCell ref="AI18:AI19"/>
+    <mergeCell ref="AI20:AJ20"/>
+    <mergeCell ref="AL16:AL21"/>
+    <mergeCell ref="AK16:AK20"/>
     <mergeCell ref="AP16:AP21"/>
     <mergeCell ref="AO16:AO21"/>
     <mergeCell ref="AN16:AN21"/>
@@ -24397,11 +24389,31 @@
     <mergeCell ref="AE16:AE20"/>
     <mergeCell ref="AM16:AM21"/>
     <mergeCell ref="AI16:AJ17"/>
-    <mergeCell ref="AJ18:AJ19"/>
-    <mergeCell ref="AI18:AI19"/>
-    <mergeCell ref="AI20:AJ20"/>
-    <mergeCell ref="AL16:AL21"/>
-    <mergeCell ref="AK16:AK20"/>
+    <mergeCell ref="Q16:Q19"/>
+    <mergeCell ref="X16:X20"/>
+    <mergeCell ref="B1:R2"/>
+    <mergeCell ref="U16:U19"/>
+    <mergeCell ref="R16:R19"/>
+    <mergeCell ref="B16:B21"/>
+    <mergeCell ref="M16:M19"/>
+    <mergeCell ref="L16:L19"/>
+    <mergeCell ref="F16:F19"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="T16:T19"/>
+    <mergeCell ref="S16:S20"/>
+    <mergeCell ref="V16:V19"/>
+    <mergeCell ref="W16:W19"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="P16:P19"/>
+    <mergeCell ref="O16:O19"/>
+    <mergeCell ref="N16:N19"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="G16:G19"/>
+    <mergeCell ref="D16:D21"/>
+    <mergeCell ref="K16:K19"/>
+    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="I16:I19"/>
+    <mergeCell ref="C16:C20"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <printOptions gridLines="1"/>
@@ -24427,7 +24439,7 @@
       <selection activeCell="D23" sqref="D23"/>
       <selection pane="topRight" activeCell="D23" sqref="D23"/>
       <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
-      <selection pane="bottomRight" activeCell="D16" sqref="D16:D21"/>
+      <selection pane="bottomRight" activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5" customHeight="1"/>
@@ -24460,21 +24472,21 @@
   <sheetData>
     <row r="1" spans="1:40" ht="13.5" customHeight="1">
       <c r="A1" s="127"/>
-      <c r="B1" s="255" t="s">
+      <c r="B1" s="250" t="s">
         <v>264</v>
       </c>
-      <c r="C1" s="255"/>
-      <c r="D1" s="255"/>
-      <c r="E1" s="255"/>
-      <c r="F1" s="255"/>
-      <c r="G1" s="255"/>
-      <c r="H1" s="255"/>
-      <c r="I1" s="255"/>
-      <c r="J1" s="255"/>
-      <c r="K1" s="255"/>
-      <c r="L1" s="255"/>
-      <c r="M1" s="255"/>
-      <c r="N1" s="255"/>
+      <c r="C1" s="250"/>
+      <c r="D1" s="250"/>
+      <c r="E1" s="250"/>
+      <c r="F1" s="250"/>
+      <c r="G1" s="250"/>
+      <c r="H1" s="250"/>
+      <c r="I1" s="250"/>
+      <c r="J1" s="250"/>
+      <c r="K1" s="250"/>
+      <c r="L1" s="250"/>
+      <c r="M1" s="250"/>
+      <c r="N1" s="250"/>
       <c r="O1" s="128"/>
       <c r="P1" s="129"/>
       <c r="Q1" s="129"/>
@@ -24504,19 +24516,19 @@
     </row>
     <row r="2" spans="1:40" ht="13.5" customHeight="1" thickBot="1">
       <c r="A2" s="135"/>
-      <c r="B2" s="256"/>
-      <c r="C2" s="256"/>
-      <c r="D2" s="256"/>
-      <c r="E2" s="256"/>
-      <c r="F2" s="256"/>
-      <c r="G2" s="256"/>
-      <c r="H2" s="256"/>
-      <c r="I2" s="256"/>
-      <c r="J2" s="256"/>
-      <c r="K2" s="256"/>
-      <c r="L2" s="256"/>
-      <c r="M2" s="256"/>
-      <c r="N2" s="256"/>
+      <c r="B2" s="251"/>
+      <c r="C2" s="251"/>
+      <c r="D2" s="251"/>
+      <c r="E2" s="251"/>
+      <c r="F2" s="251"/>
+      <c r="G2" s="251"/>
+      <c r="H2" s="251"/>
+      <c r="I2" s="251"/>
+      <c r="J2" s="251"/>
+      <c r="K2" s="251"/>
+      <c r="L2" s="251"/>
+      <c r="M2" s="251"/>
+      <c r="N2" s="251"/>
       <c r="O2" s="31"/>
       <c r="S2" s="33"/>
       <c r="T2" s="33"/>
@@ -24733,14 +24745,14 @@
       <c r="K9" s="33" t="s">
         <v>265</v>
       </c>
-      <c r="R9" s="238" t="s">
+      <c r="R9" s="247" t="s">
         <v>158</v>
       </c>
-      <c r="S9" s="238"/>
-      <c r="T9" s="238"/>
-      <c r="U9" s="238"/>
-      <c r="V9" s="238"/>
-      <c r="W9" s="238"/>
+      <c r="S9" s="247"/>
+      <c r="T9" s="247"/>
+      <c r="U9" s="247"/>
+      <c r="V9" s="247"/>
+      <c r="W9" s="247"/>
       <c r="Z9" s="62"/>
       <c r="AA9" s="58"/>
       <c r="AB9" s="58"/>
@@ -24772,12 +24784,12 @@
       <c r="K10" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="R10" s="238"/>
-      <c r="S10" s="238"/>
-      <c r="T10" s="238"/>
-      <c r="U10" s="238"/>
-      <c r="V10" s="238"/>
-      <c r="W10" s="238"/>
+      <c r="R10" s="247"/>
+      <c r="S10" s="247"/>
+      <c r="T10" s="247"/>
+      <c r="U10" s="247"/>
+      <c r="V10" s="247"/>
+      <c r="W10" s="247"/>
       <c r="Z10" s="62"/>
       <c r="AD10" s="30"/>
       <c r="AE10" s="32"/>
@@ -24905,12 +24917,12 @@
       </c>
       <c r="Y14" s="34"/>
       <c r="Z14" s="34"/>
-      <c r="AE14" s="249" t="s">
+      <c r="AE14" s="255" t="s">
         <v>373</v>
       </c>
-      <c r="AF14" s="250"/>
-      <c r="AG14" s="250"/>
-      <c r="AH14" s="251"/>
+      <c r="AF14" s="256"/>
+      <c r="AG14" s="256"/>
+      <c r="AH14" s="257"/>
       <c r="AM14" s="136"/>
       <c r="AN14" s="121"/>
     </row>
@@ -24919,117 +24931,117 @@
       <c r="O15" s="35"/>
       <c r="P15" s="35"/>
       <c r="Q15" s="35"/>
-      <c r="AE15" s="252" t="s">
+      <c r="AE15" s="258" t="s">
         <v>374</v>
       </c>
-      <c r="AF15" s="253"/>
-      <c r="AG15" s="253"/>
-      <c r="AH15" s="254"/>
+      <c r="AF15" s="259"/>
+      <c r="AG15" s="259"/>
+      <c r="AH15" s="260"/>
       <c r="AM15" s="136"/>
       <c r="AN15" s="121"/>
     </row>
     <row r="16" spans="1:40" ht="13.5" customHeight="1">
-      <c r="A16" s="248" t="s">
+      <c r="A16" s="235" t="s">
         <v>263</v>
       </c>
-      <c r="B16" s="235" t="s">
+      <c r="B16" s="236" t="s">
         <v>253</v>
       </c>
-      <c r="C16" s="235" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="235" t="s">
+      <c r="C16" s="236" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="236" t="s">
         <v>99</v>
       </c>
-      <c r="E16" s="235" t="s">
+      <c r="E16" s="236" t="s">
         <v>145</v>
       </c>
-      <c r="F16" s="235" t="s">
+      <c r="F16" s="236" t="s">
         <v>144</v>
       </c>
-      <c r="G16" s="257" t="s">
+      <c r="G16" s="252" t="s">
         <v>376</v>
       </c>
-      <c r="H16" s="235" t="s">
-        <v>269</v>
-      </c>
-      <c r="I16" s="235" t="s">
-        <v>270</v>
-      </c>
-      <c r="J16" s="235" t="s">
-        <v>267</v>
-      </c>
-      <c r="K16" s="235" t="s">
-        <v>268</v>
-      </c>
-      <c r="L16" s="235" t="s">
+      <c r="H16" s="236" t="s">
+        <v>409</v>
+      </c>
+      <c r="I16" s="236" t="s">
+        <v>410</v>
+      </c>
+      <c r="J16" s="236" t="s">
+        <v>411</v>
+      </c>
+      <c r="K16" s="236" t="s">
+        <v>412</v>
+      </c>
+      <c r="L16" s="236" t="s">
         <v>146</v>
       </c>
-      <c r="M16" s="235" t="s">
+      <c r="M16" s="236" t="s">
         <v>146</v>
       </c>
-      <c r="N16" s="235" t="s">
+      <c r="N16" s="236" t="s">
         <v>274</v>
       </c>
-      <c r="O16" s="239" t="s">
+      <c r="O16" s="237" t="s">
         <v>147</v>
       </c>
-      <c r="P16" s="239" t="s">
+      <c r="P16" s="237" t="s">
         <v>304</v>
       </c>
-      <c r="Q16" s="239" t="s">
+      <c r="Q16" s="237" t="s">
         <v>334</v>
       </c>
-      <c r="R16" s="240" t="s">
+      <c r="R16" s="248" t="s">
         <v>135</v>
       </c>
-      <c r="S16" s="235" t="s">
+      <c r="S16" s="236" t="s">
         <v>136</v>
       </c>
-      <c r="T16" s="235" t="s">
+      <c r="T16" s="236" t="s">
         <v>137</v>
       </c>
-      <c r="U16" s="235" t="s">
+      <c r="U16" s="236" t="s">
         <v>368</v>
       </c>
-      <c r="V16" s="235" t="s">
+      <c r="V16" s="236" t="s">
         <v>138</v>
       </c>
-      <c r="W16" s="235" t="s">
+      <c r="W16" s="236" t="s">
         <v>139</v>
       </c>
-      <c r="X16" s="235" t="s">
+      <c r="X16" s="236" t="s">
         <v>140</v>
       </c>
-      <c r="Y16" s="235" t="s">
+      <c r="Y16" s="236" t="s">
         <v>141</v>
       </c>
-      <c r="Z16" s="235" t="s">
+      <c r="Z16" s="236" t="s">
         <v>142</v>
       </c>
-      <c r="AA16" s="235" t="s">
+      <c r="AA16" s="236" t="s">
         <v>370</v>
       </c>
-      <c r="AB16" s="235" t="s">
+      <c r="AB16" s="236" t="s">
         <v>330</v>
       </c>
-      <c r="AC16" s="235"/>
-      <c r="AD16" s="235" t="s">
+      <c r="AC16" s="236"/>
+      <c r="AD16" s="236" t="s">
         <v>282</v>
       </c>
-      <c r="AE16" s="260" t="s">
+      <c r="AE16" s="249" t="s">
         <v>68</v>
       </c>
-      <c r="AF16" s="260" t="s">
+      <c r="AF16" s="249" t="s">
         <v>69</v>
       </c>
-      <c r="AG16" s="260" t="s">
+      <c r="AG16" s="249" t="s">
         <v>159</v>
       </c>
-      <c r="AH16" s="260" t="s">
+      <c r="AH16" s="249" t="s">
         <v>160</v>
       </c>
-      <c r="AI16" s="237" t="s">
+      <c r="AI16" s="245" t="s">
         <v>108</v>
       </c>
       <c r="AJ16" s="42"/>
@@ -25037,134 +25049,134 @@
       <c r="AN16" s="121"/>
     </row>
     <row r="17" spans="1:40" ht="13.5" customHeight="1">
-      <c r="A17" s="248"/>
-      <c r="B17" s="235"/>
-      <c r="C17" s="235"/>
-      <c r="D17" s="235"/>
-      <c r="E17" s="235"/>
-      <c r="F17" s="235"/>
-      <c r="G17" s="258"/>
-      <c r="H17" s="235"/>
-      <c r="I17" s="235"/>
-      <c r="J17" s="235"/>
-      <c r="K17" s="235"/>
-      <c r="L17" s="235"/>
-      <c r="M17" s="235"/>
-      <c r="N17" s="235"/>
-      <c r="O17" s="239"/>
-      <c r="P17" s="239"/>
-      <c r="Q17" s="239"/>
-      <c r="R17" s="240"/>
-      <c r="S17" s="235"/>
-      <c r="T17" s="235"/>
-      <c r="U17" s="235"/>
-      <c r="V17" s="235"/>
-      <c r="W17" s="235"/>
-      <c r="X17" s="235"/>
-      <c r="Y17" s="235"/>
-      <c r="Z17" s="235"/>
-      <c r="AA17" s="235"/>
-      <c r="AB17" s="235"/>
-      <c r="AC17" s="235"/>
-      <c r="AD17" s="235"/>
-      <c r="AE17" s="260"/>
-      <c r="AF17" s="260"/>
-      <c r="AG17" s="260"/>
-      <c r="AH17" s="260"/>
-      <c r="AI17" s="237"/>
+      <c r="A17" s="235"/>
+      <c r="B17" s="236"/>
+      <c r="C17" s="236"/>
+      <c r="D17" s="236"/>
+      <c r="E17" s="236"/>
+      <c r="F17" s="236"/>
+      <c r="G17" s="253"/>
+      <c r="H17" s="236"/>
+      <c r="I17" s="236"/>
+      <c r="J17" s="236"/>
+      <c r="K17" s="236"/>
+      <c r="L17" s="236"/>
+      <c r="M17" s="236"/>
+      <c r="N17" s="236"/>
+      <c r="O17" s="237"/>
+      <c r="P17" s="237"/>
+      <c r="Q17" s="237"/>
+      <c r="R17" s="248"/>
+      <c r="S17" s="236"/>
+      <c r="T17" s="236"/>
+      <c r="U17" s="236"/>
+      <c r="V17" s="236"/>
+      <c r="W17" s="236"/>
+      <c r="X17" s="236"/>
+      <c r="Y17" s="236"/>
+      <c r="Z17" s="236"/>
+      <c r="AA17" s="236"/>
+      <c r="AB17" s="236"/>
+      <c r="AC17" s="236"/>
+      <c r="AD17" s="236"/>
+      <c r="AE17" s="249"/>
+      <c r="AF17" s="249"/>
+      <c r="AG17" s="249"/>
+      <c r="AH17" s="249"/>
+      <c r="AI17" s="245"/>
       <c r="AJ17" s="42"/>
       <c r="AM17" s="136"/>
       <c r="AN17" s="121"/>
     </row>
     <row r="18" spans="1:40" ht="13.5" customHeight="1">
-      <c r="A18" s="248"/>
-      <c r="B18" s="235"/>
-      <c r="C18" s="235"/>
-      <c r="D18" s="235"/>
-      <c r="E18" s="235"/>
-      <c r="F18" s="235"/>
-      <c r="G18" s="258"/>
-      <c r="H18" s="235"/>
-      <c r="I18" s="235"/>
-      <c r="J18" s="235"/>
-      <c r="K18" s="235"/>
-      <c r="L18" s="235"/>
-      <c r="M18" s="235"/>
-      <c r="N18" s="235"/>
-      <c r="O18" s="239"/>
-      <c r="P18" s="239"/>
-      <c r="Q18" s="239"/>
-      <c r="R18" s="240"/>
-      <c r="S18" s="235"/>
-      <c r="T18" s="235"/>
-      <c r="U18" s="235"/>
-      <c r="V18" s="235"/>
-      <c r="W18" s="235"/>
-      <c r="X18" s="235"/>
-      <c r="Y18" s="235"/>
-      <c r="Z18" s="235"/>
-      <c r="AA18" s="235"/>
-      <c r="AB18" s="235" t="s">
+      <c r="A18" s="235"/>
+      <c r="B18" s="236"/>
+      <c r="C18" s="236"/>
+      <c r="D18" s="236"/>
+      <c r="E18" s="236"/>
+      <c r="F18" s="236"/>
+      <c r="G18" s="253"/>
+      <c r="H18" s="236"/>
+      <c r="I18" s="236"/>
+      <c r="J18" s="236"/>
+      <c r="K18" s="236"/>
+      <c r="L18" s="236"/>
+      <c r="M18" s="236"/>
+      <c r="N18" s="236"/>
+      <c r="O18" s="237"/>
+      <c r="P18" s="237"/>
+      <c r="Q18" s="237"/>
+      <c r="R18" s="248"/>
+      <c r="S18" s="236"/>
+      <c r="T18" s="236"/>
+      <c r="U18" s="236"/>
+      <c r="V18" s="236"/>
+      <c r="W18" s="236"/>
+      <c r="X18" s="236"/>
+      <c r="Y18" s="236"/>
+      <c r="Z18" s="236"/>
+      <c r="AA18" s="236"/>
+      <c r="AB18" s="236" t="s">
         <v>322</v>
       </c>
-      <c r="AC18" s="235" t="s">
+      <c r="AC18" s="236" t="s">
         <v>323</v>
       </c>
-      <c r="AD18" s="235"/>
-      <c r="AE18" s="260"/>
-      <c r="AF18" s="260"/>
-      <c r="AG18" s="260"/>
-      <c r="AH18" s="260"/>
-      <c r="AI18" s="237"/>
+      <c r="AD18" s="236"/>
+      <c r="AE18" s="249"/>
+      <c r="AF18" s="249"/>
+      <c r="AG18" s="249"/>
+      <c r="AH18" s="249"/>
+      <c r="AI18" s="245"/>
       <c r="AJ18" s="42"/>
       <c r="AM18" s="136"/>
       <c r="AN18" s="121"/>
     </row>
     <row r="19" spans="1:40" ht="13.5" customHeight="1">
-      <c r="A19" s="248"/>
-      <c r="B19" s="235"/>
-      <c r="C19" s="235"/>
-      <c r="D19" s="235"/>
-      <c r="E19" s="235"/>
-      <c r="F19" s="235"/>
-      <c r="G19" s="259"/>
-      <c r="H19" s="235"/>
-      <c r="I19" s="235"/>
-      <c r="J19" s="235"/>
-      <c r="K19" s="235"/>
-      <c r="L19" s="235"/>
-      <c r="M19" s="235"/>
-      <c r="N19" s="235"/>
-      <c r="O19" s="239"/>
-      <c r="P19" s="239"/>
-      <c r="Q19" s="239"/>
-      <c r="R19" s="240"/>
-      <c r="S19" s="235"/>
-      <c r="T19" s="235"/>
-      <c r="U19" s="235"/>
-      <c r="V19" s="235"/>
-      <c r="W19" s="235"/>
-      <c r="X19" s="235"/>
-      <c r="Y19" s="235"/>
-      <c r="Z19" s="235"/>
-      <c r="AA19" s="235"/>
-      <c r="AB19" s="235"/>
-      <c r="AC19" s="235"/>
-      <c r="AD19" s="235"/>
-      <c r="AE19" s="260"/>
-      <c r="AF19" s="260"/>
-      <c r="AG19" s="260"/>
-      <c r="AH19" s="260"/>
-      <c r="AI19" s="237"/>
+      <c r="A19" s="235"/>
+      <c r="B19" s="236"/>
+      <c r="C19" s="236"/>
+      <c r="D19" s="236"/>
+      <c r="E19" s="236"/>
+      <c r="F19" s="236"/>
+      <c r="G19" s="254"/>
+      <c r="H19" s="236"/>
+      <c r="I19" s="236"/>
+      <c r="J19" s="236"/>
+      <c r="K19" s="236"/>
+      <c r="L19" s="236"/>
+      <c r="M19" s="236"/>
+      <c r="N19" s="236"/>
+      <c r="O19" s="237"/>
+      <c r="P19" s="237"/>
+      <c r="Q19" s="237"/>
+      <c r="R19" s="248"/>
+      <c r="S19" s="236"/>
+      <c r="T19" s="236"/>
+      <c r="U19" s="236"/>
+      <c r="V19" s="236"/>
+      <c r="W19" s="236"/>
+      <c r="X19" s="236"/>
+      <c r="Y19" s="236"/>
+      <c r="Z19" s="236"/>
+      <c r="AA19" s="236"/>
+      <c r="AB19" s="236"/>
+      <c r="AC19" s="236"/>
+      <c r="AD19" s="236"/>
+      <c r="AE19" s="249"/>
+      <c r="AF19" s="249"/>
+      <c r="AG19" s="249"/>
+      <c r="AH19" s="249"/>
+      <c r="AI19" s="245"/>
       <c r="AJ19" s="42"/>
       <c r="AM19" s="136"/>
       <c r="AN19" s="121"/>
     </row>
     <row r="20" spans="1:40" ht="13.5" customHeight="1">
-      <c r="A20" s="248"/>
-      <c r="B20" s="235"/>
-      <c r="C20" s="235"/>
-      <c r="D20" s="235"/>
+      <c r="A20" s="235"/>
+      <c r="B20" s="236"/>
+      <c r="C20" s="236"/>
+      <c r="D20" s="236"/>
       <c r="E20" s="177" t="s">
         <v>149</v>
       </c>
@@ -25193,40 +25205,40 @@
       <c r="N20" s="177" t="s">
         <v>276</v>
       </c>
-      <c r="O20" s="239"/>
+      <c r="O20" s="237"/>
       <c r="P20" s="178" t="s">
         <v>151</v>
       </c>
-      <c r="Q20" s="239"/>
-      <c r="R20" s="240"/>
-      <c r="S20" s="235"/>
-      <c r="T20" s="235"/>
-      <c r="U20" s="235"/>
-      <c r="V20" s="235"/>
-      <c r="W20" s="235"/>
-      <c r="X20" s="235"/>
-      <c r="Y20" s="235"/>
-      <c r="Z20" s="235"/>
-      <c r="AA20" s="235"/>
-      <c r="AB20" s="235"/>
-      <c r="AC20" s="235"/>
-      <c r="AD20" s="235"/>
-      <c r="AE20" s="260"/>
-      <c r="AF20" s="260"/>
-      <c r="AG20" s="260"/>
-      <c r="AH20" s="260"/>
-      <c r="AI20" s="237"/>
+      <c r="Q20" s="237"/>
+      <c r="R20" s="248"/>
+      <c r="S20" s="236"/>
+      <c r="T20" s="236"/>
+      <c r="U20" s="236"/>
+      <c r="V20" s="236"/>
+      <c r="W20" s="236"/>
+      <c r="X20" s="236"/>
+      <c r="Y20" s="236"/>
+      <c r="Z20" s="236"/>
+      <c r="AA20" s="236"/>
+      <c r="AB20" s="236"/>
+      <c r="AC20" s="236"/>
+      <c r="AD20" s="236"/>
+      <c r="AE20" s="249"/>
+      <c r="AF20" s="249"/>
+      <c r="AG20" s="249"/>
+      <c r="AH20" s="249"/>
+      <c r="AI20" s="245"/>
       <c r="AJ20" s="42"/>
       <c r="AM20" s="136"/>
       <c r="AN20" s="121"/>
     </row>
     <row r="21" spans="1:40" s="32" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A21" s="248"/>
-      <c r="B21" s="235"/>
+      <c r="A21" s="235"/>
+      <c r="B21" s="236"/>
       <c r="C21" s="177">
         <v>3019</v>
       </c>
-      <c r="D21" s="235"/>
+      <c r="D21" s="236"/>
       <c r="E21" s="177"/>
       <c r="F21" s="44">
         <v>395</v>
@@ -25287,11 +25299,11 @@
       <c r="AD21" s="177">
         <v>1069</v>
       </c>
-      <c r="AE21" s="260"/>
-      <c r="AF21" s="260"/>
-      <c r="AG21" s="260"/>
-      <c r="AH21" s="260"/>
-      <c r="AI21" s="237"/>
+      <c r="AE21" s="249"/>
+      <c r="AF21" s="249"/>
+      <c r="AG21" s="249"/>
+      <c r="AH21" s="249"/>
+      <c r="AI21" s="245"/>
       <c r="AJ21" s="42"/>
       <c r="AM21" s="137"/>
       <c r="AN21" s="122"/>
@@ -42642,31 +42654,6 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="AD16:AD20"/>
-    <mergeCell ref="AE16:AE21"/>
-    <mergeCell ref="AG16:AG21"/>
-    <mergeCell ref="AH16:AH21"/>
-    <mergeCell ref="AI16:AI21"/>
-    <mergeCell ref="AF16:AF21"/>
-    <mergeCell ref="W16:W20"/>
-    <mergeCell ref="X16:X20"/>
-    <mergeCell ref="Z16:Z20"/>
-    <mergeCell ref="AA16:AA20"/>
-    <mergeCell ref="AB16:AC17"/>
-    <mergeCell ref="AB18:AB19"/>
-    <mergeCell ref="AC18:AC19"/>
-    <mergeCell ref="AB20:AC20"/>
-    <mergeCell ref="Q16:Q20"/>
-    <mergeCell ref="R16:R20"/>
-    <mergeCell ref="S16:S20"/>
-    <mergeCell ref="T16:T20"/>
-    <mergeCell ref="V16:V20"/>
-    <mergeCell ref="B1:N2"/>
-    <mergeCell ref="K16:K19"/>
-    <mergeCell ref="L16:L19"/>
-    <mergeCell ref="M16:M19"/>
-    <mergeCell ref="N16:N19"/>
-    <mergeCell ref="G16:G19"/>
     <mergeCell ref="AE14:AH14"/>
     <mergeCell ref="AE15:AH15"/>
     <mergeCell ref="R9:W10"/>
@@ -42683,6 +42670,31 @@
     <mergeCell ref="Y16:Y20"/>
     <mergeCell ref="U16:U20"/>
     <mergeCell ref="P16:P19"/>
+    <mergeCell ref="B1:N2"/>
+    <mergeCell ref="K16:K19"/>
+    <mergeCell ref="L16:L19"/>
+    <mergeCell ref="M16:M19"/>
+    <mergeCell ref="N16:N19"/>
+    <mergeCell ref="G16:G19"/>
+    <mergeCell ref="Q16:Q20"/>
+    <mergeCell ref="R16:R20"/>
+    <mergeCell ref="S16:S20"/>
+    <mergeCell ref="T16:T20"/>
+    <mergeCell ref="V16:V20"/>
+    <mergeCell ref="W16:W20"/>
+    <mergeCell ref="X16:X20"/>
+    <mergeCell ref="Z16:Z20"/>
+    <mergeCell ref="AA16:AA20"/>
+    <mergeCell ref="AB16:AC17"/>
+    <mergeCell ref="AB18:AB19"/>
+    <mergeCell ref="AC18:AC19"/>
+    <mergeCell ref="AB20:AC20"/>
+    <mergeCell ref="AD16:AD20"/>
+    <mergeCell ref="AE16:AE21"/>
+    <mergeCell ref="AG16:AG21"/>
+    <mergeCell ref="AH16:AH21"/>
+    <mergeCell ref="AI16:AI21"/>
+    <mergeCell ref="AF16:AF21"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.75" header="0.3" footer="0.3"/>
@@ -50206,44 +50218,44 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6531C455-43DF-4518-B2DB-CCE28F0AF57B}" fitToPage="1" showRuler="0">
+    <customSheetView guid="{F6426E77-C675-444E-AC8D-180F66AA3059}" fitToPage="1" showRuler="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup scale="70" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{52161C46-7293-49CA-889B-1A1303EEF9B9}" fitToPage="1" showRuler="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="A67" sqref="A67"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup scale="70" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+      <pageSetup scale="70" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{9D9E1FF7-61E9-4438-AEF2-B8A5765BA2AD}" fitToPage="1" showRuler="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="A67" sqref="A67"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup scale="70" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+      <headerFooter alignWithMargins="0"/>
+    </customSheetView>
+    <customSheetView guid="{F566A51D-D37D-4C9A-A044-3E5B85972913}" fitToPage="1" showRuler="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="B65" sqref="B65"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup scale="70" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
     <customSheetView guid="{7A3CD00D-9588-4788-B636-9D2E31C8323F}" fitToPage="1" showRuler="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="A67" sqref="A67"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup scale="70" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{F566A51D-D37D-4C9A-A044-3E5B85972913}" fitToPage="1" showRuler="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="B65" sqref="B65"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup scale="70" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{9D9E1FF7-61E9-4438-AEF2-B8A5765BA2AD}" fitToPage="1" showRuler="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="A67" sqref="A67"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-      <pageSetup scale="70" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
-      <headerFooter alignWithMargins="0"/>
-    </customSheetView>
-    <customSheetView guid="{52161C46-7293-49CA-889B-1A1303EEF9B9}" fitToPage="1" showRuler="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="A67" sqref="A67"/>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup scale="70" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId5"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{F6426E77-C675-444E-AC8D-180F66AA3059}" fitToPage="1" showRuler="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+    <customSheetView guid="{6531C455-43DF-4518-B2DB-CCE28F0AF57B}" fitToPage="1" showRuler="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="A67" sqref="A67"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup scale="70" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId6"/>
       <headerFooter alignWithMargins="0"/>

</xml_diff>